<commit_message>
First round of commits
</commit_message>
<xml_diff>
--- a/Master SKU List.xlsx
+++ b/Master SKU List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heeva\Dropbox\Cal Poly SOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smarnita/Documents/flushPackagingProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7EB0E6-2560-40FB-BF81-34188E9DE969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F18B46-8771-934A-9967-B386B5AF41A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94C1B0B8-171D-4CFE-BFDD-04552866E740}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{94C1B0B8-171D-4CFE-BFDD-04552866E740}"/>
   </bookViews>
   <sheets>
     <sheet name="Flush Product Listings" sheetId="11" r:id="rId1"/>
@@ -2588,50 +2588,49 @@
   <dimension ref="A1:AM165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5" style="2" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.5" style="2" customWidth="1"/>
     <col min="20" max="21" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.5" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5" style="2" customWidth="1"/>
+    <col min="27" max="27" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.5" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="2"/>
+    <col min="32" max="32" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="34.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>341</v>
       </c>

</xml_diff>